<commit_message>
Adde LLM testing and fixed other code
</commit_message>
<xml_diff>
--- a/src/langchain_code/resultts/r1/Results.xlsx
+++ b/src/langchain_code/resultts/r1/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Local Disk D\Capstone Sartaj branch\Resonate\src\langchain_code\resultts\r1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A1E57-02C0-4A05-B277-C56B13753279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F6D0EB7-A9BA-4454-B21D-F9CF6B5CA116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{36FC2D4D-A66F-4BD3-BBC5-5F1DBFFC87BD}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="60">
   <si>
     <t>Memory</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">color is not good idea, thinner lines, use different marker, disk, X, squere markers, use markers instead of color. </t>
   </si>
 </sst>
 </file>
@@ -295,7 +298,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -309,13 +312,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-IN"/>
-              <a:t>Tokens</a:t>
+              <a:t>Tokens Spent</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-IN" baseline="0"/>
-              <a:t> Spent</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-IN"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -332,7 +330,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -369,7 +367,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -378,8 +376,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -388,15 +386,16 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Tokens Spent'!$B$1:$AY$1</c:f>
+              <c:f>'Tokens Spent'!$B$1:$Z$1</c:f>
               <c:strCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>Q1</c:v>
                 </c:pt>
@@ -471,91 +470,16 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>Q25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Q26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Q27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Q28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Q29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Q30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Q31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Q32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Q33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Q34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Q35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Q36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Q37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Q38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Q39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Q40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Q41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Q42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Q43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Q44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Q45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Q46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Q47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Q48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Q49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Q50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tokens Spent'!$B$2:$AY$2</c:f>
+              <c:f>'Tokens Spent'!$B$2:$Z$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>5160</c:v>
                 </c:pt>
@@ -596,7 +520,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -605,8 +529,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -615,15 +539,16 @@
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Tokens Spent'!$B$1:$AY$1</c:f>
+              <c:f>'Tokens Spent'!$B$1:$Z$1</c:f>
               <c:strCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>Q1</c:v>
                 </c:pt>
@@ -698,91 +623,16 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>Q25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Q26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Q27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Q28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Q29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Q30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Q31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Q32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Q33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Q34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Q35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Q36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Q37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Q38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Q39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Q40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Q41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Q42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Q43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Q44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Q45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Q46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Q47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Q48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Q49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Q50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tokens Spent'!$B$3:$AY$3</c:f>
+              <c:f>'Tokens Spent'!$B$3:$Z$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>5160</c:v>
                 </c:pt>
@@ -856,7 +706,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -865,8 +715,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
@@ -875,15 +725,16 @@
                 <a:solidFill>
                   <a:schemeClr val="accent3"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Tokens Spent'!$B$1:$AY$1</c:f>
+              <c:f>'Tokens Spent'!$B$1:$Z$1</c:f>
               <c:strCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>Q1</c:v>
                 </c:pt>
@@ -958,91 +809,16 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>Q25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Q26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Q27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Q28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Q29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Q30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Q31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Q32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Q33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Q34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Q35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Q36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Q37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Q38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Q39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Q40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Q41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Q42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Q43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Q44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Q45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Q46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Q47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Q48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Q49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Q50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tokens Spent'!$B$4:$AY$4</c:f>
+              <c:f>'Tokens Spent'!$B$4:$Z$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>5160</c:v>
                 </c:pt>
@@ -1083,7 +859,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -1092,25 +868,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Tokens Spent'!$B$1:$AY$1</c:f>
+              <c:f>'Tokens Spent'!$B$1:$Z$1</c:f>
               <c:strCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>Q1</c:v>
                 </c:pt>
@@ -1185,91 +960,16 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>Q25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Q26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Q27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Q28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Q29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Q30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Q31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Q32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Q33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Q34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Q35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Q36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Q37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Q38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Q39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Q40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Q41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Q42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Q43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Q44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Q45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Q46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Q47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Q48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Q49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Q50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tokens Spent'!$B$5:$AY$5</c:f>
+              <c:f>'Tokens Spent'!$B$5:$Z$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>10454</c:v>
                 </c:pt>
@@ -1344,81 +1044,6 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>4331</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>10065</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>15496</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>11026</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>7608</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>6350</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>9693</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9820</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>13507</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>11220</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>11418</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8791</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9416</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>10315</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7901</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>10158</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>10379</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>11946</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>10857</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>13813</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>11581</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>11741</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9199</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>9700</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>7772</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>10689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1445,7 +1070,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -1454,25 +1079,24 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent5"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Tokens Spent'!$B$1:$AY$1</c:f>
+              <c:f>'Tokens Spent'!$B$1:$Z$1</c:f>
               <c:strCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>Q1</c:v>
                 </c:pt>
@@ -1547,91 +1171,16 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>Q25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Q26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Q27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Q28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Q29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Q30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Q31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Q32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Q33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Q34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Q35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Q36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Q37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Q38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Q39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Q40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Q41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Q42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Q43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Q44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Q45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Q46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Q47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Q48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Q49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Q50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tokens Spent'!$B$6:$AY$6</c:f>
+              <c:f>'Tokens Spent'!$B$6:$Z$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>10475</c:v>
                 </c:pt>
@@ -1706,81 +1255,6 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>5471</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>11234</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>16799</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>12743</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9066</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>6504</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>9938</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9945</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>13994</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>10905</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>10966</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8460</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>8822</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9587</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7127</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9380</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9195</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>10264</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>9652</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>14198</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>11718</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>11779</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9271</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>8688</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>6682</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>9469</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1807,7 +1281,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -1817,7 +1291,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1826,15 +1300,16 @@
                 <a:solidFill>
                   <a:schemeClr val="accent6"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Tokens Spent'!$B$1:$AY$1</c:f>
+              <c:f>'Tokens Spent'!$B$1:$Z$1</c:f>
               <c:strCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>Q1</c:v>
                 </c:pt>
@@ -1909,91 +1384,16 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>Q25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Q26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Q27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Q28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Q29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Q30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Q31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Q32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Q33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Q34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Q35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Q36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Q37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Q38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Q39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Q40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Q41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Q42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Q43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Q44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Q45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Q46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Q47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Q48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Q49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Q50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tokens Spent'!$B$7:$AY$7</c:f>
+              <c:f>'Tokens Spent'!$B$7:$Z$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>10463</c:v>
                 </c:pt>
@@ -2068,81 +1468,6 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2966</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>8434</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13432</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8777</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6565</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7140</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>10648</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>10908</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>14532</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>11255</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>11246</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8675</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9438</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>10282</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7853</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9651</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>8586</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>9936</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>9687</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>14392</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>12389</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>12373</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9602</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>10139</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>8241</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>11119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2169,7 +1494,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
@@ -2180,29 +1505,26 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:lumMod val="60000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent1">
                     <a:lumMod val="60000"/>
                   </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'Tokens Spent'!$B$1:$AY$1</c:f>
+              <c:f>'Tokens Spent'!$B$1:$Z$1</c:f>
               <c:strCache>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>Q1</c:v>
                 </c:pt>
@@ -2277,91 +1599,16 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>Q25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>Q26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>Q27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>Q28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>Q29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>Q30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>Q31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>Q32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>Q33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>Q34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>Q35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>Q36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>Q37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>Q38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>Q39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>Q40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>Q41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>Q42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>Q43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>Q44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>Q45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>Q46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>Q47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>Q48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>Q49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>Q50</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Tokens Spent'!$B$8:$AY$8</c:f>
+              <c:f>'Tokens Spent'!$B$8:$Z$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>10446</c:v>
                 </c:pt>
@@ -2436,81 +1683,6 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2915</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>8427</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>13495</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8909</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6663</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>10244</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>10512</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>15005</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>12792</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>11465</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8714</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9137</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9814</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>7231</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9664</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>10005</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>11030</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>9655</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>14170</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>11759</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>11898</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9418</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>9783</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>7678</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>10288</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2542,6 +1714,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2564,7 +1750,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2593,28 +1779,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2651,7 +1829,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2694,7 +1872,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2766,7 +1944,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2777,7 +1955,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2800,18 +1978,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -2823,7 +2001,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2831,11 +2009,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -2867,35 +2045,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2907,30 +2095,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2952,15 +2144,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2975,15 +2165,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2994,17 +2184,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -3013,10 +2202,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -3032,21 +2221,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -3065,17 +2248,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -3084,17 +2266,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -3103,17 +2284,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -3134,7 +2314,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -3142,7 +2322,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -3155,6 +2335,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -3162,10 +2353,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -3186,7 +2377,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -3195,14 +2386,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -3216,7 +2407,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -3232,8 +2423,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3249,6 +2440,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3256,14 +2458,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3275,13 +2471,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>1120140</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
       <xdr:colOff>68580</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3626,10 +2822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBFB2D52-CC40-4E64-95D3-96029CA4C46D}">
-  <dimension ref="A1:AY8"/>
+  <dimension ref="A1:AY10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB10" sqref="AB10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3642,17 +2838,21 @@
     <col min="9" max="12" width="6" bestFit="1" customWidth="1"/>
     <col min="13" max="15" width="5" bestFit="1" customWidth="1"/>
     <col min="16" max="19" width="6" bestFit="1" customWidth="1"/>
-    <col min="20" max="23" width="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="6" bestFit="1" customWidth="1"/>
     <col min="25" max="26" width="5" bestFit="1" customWidth="1"/>
     <col min="27" max="29" width="6" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="6" bestFit="1" customWidth="1"/>
+    <col min="30" max="31" width="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="36" width="6" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="5" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="6" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="5" bestFit="1" customWidth="1"/>
     <col min="41" max="47" width="6" bestFit="1" customWidth="1"/>
-    <col min="48" max="50" width="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="6" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5" bestFit="1" customWidth="1"/>
     <col min="51" max="52" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4522,6 +3722,11 @@
       </c>
       <c r="AY8">
         <v>10288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -4535,8 +3740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3930C51C-B68D-4E30-9E4F-9CE40A19BCD8}">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54:G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5349,31 +4554,31 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
-        <f>SUM(A2:A52)</f>
+        <f t="shared" ref="A54:G54" si="0">SUM(A2:A52)</f>
         <v>8.4057999999999897E-2</v>
       </c>
       <c r="B54">
-        <f>SUM(B2:B52)</f>
+        <f t="shared" si="0"/>
         <v>0.23568349999999991</v>
       </c>
       <c r="C54">
-        <f>SUM(C2:C52)</f>
+        <f t="shared" si="0"/>
         <v>8.4067999999999893E-2</v>
       </c>
       <c r="D54">
-        <f>SUM(D2:D52)</f>
+        <f t="shared" si="0"/>
         <v>0.72177749999999985</v>
       </c>
       <c r="E54">
-        <f>SUM(E2:E52)</f>
+        <f t="shared" si="0"/>
         <v>0.7095534999999995</v>
       </c>
       <c r="F54">
-        <f>SUM(F2:F52)</f>
+        <f t="shared" si="0"/>
         <v>0.69188299999999991</v>
       </c>
       <c r="G54">
-        <f>SUM(G2:G52)</f>
+        <f t="shared" si="0"/>
         <v>0.71032399999999973</v>
       </c>
       <c r="H54" t="s">

</xml_diff>